<commit_message>
Updating Master League files
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Master - Season 01.xlsx
+++ b/src/main/resources/data/Master - Season 01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpaces\workspace estudo\pokemonGoPvpAnalyzer\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A47119-3F45-407C-9516-ECBCBF3C2CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC303AB-8FCB-4559-9F79-15A95B1F2737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{68075319-8292-4D77-A75F-91AD9F2E35E0}"/>
+    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{68075319-8292-4D77-A75F-91AD9F2E35E0}"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="7" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="284">
   <si>
     <t>Lead</t>
   </si>
@@ -835,6 +835,75 @@
   </si>
   <si>
     <t>cofagrigus</t>
+  </si>
+  <si>
+    <t>Mewtwo</t>
+  </si>
+  <si>
+    <t>Melmetal</t>
+  </si>
+  <si>
+    <t>Swampert</t>
+  </si>
+  <si>
+    <t>Machamp</t>
+  </si>
+  <si>
+    <t>Metagross</t>
+  </si>
+  <si>
+    <t>Dragonite</t>
+  </si>
+  <si>
+    <t>Kyogre</t>
+  </si>
+  <si>
+    <t>Mamoswine</t>
+  </si>
+  <si>
+    <t>Dialga</t>
+  </si>
+  <si>
+    <t>Togekiss</t>
+  </si>
+  <si>
+    <t>Snorlax</t>
+  </si>
+  <si>
+    <t>Giratina_origin</t>
+  </si>
+  <si>
+    <t>Rhyperior</t>
+  </si>
+  <si>
+    <t>Tyranitar</t>
+  </si>
+  <si>
+    <t>Giratina_altered</t>
+  </si>
+  <si>
+    <t>Excadrill</t>
+  </si>
+  <si>
+    <t>Hydreigon</t>
+  </si>
+  <si>
+    <t>Glaceon</t>
+  </si>
+  <si>
+    <t>Heatran</t>
+  </si>
+  <si>
+    <t>Garchomp</t>
+  </si>
+  <si>
+    <t>Lucario</t>
+  </si>
+  <si>
+    <t>Darkrai</t>
+  </si>
+  <si>
+    <t>Gyarados</t>
   </si>
 </sst>
 </file>
@@ -920,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -930,7 +999,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1245,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CDF088-F31A-4ECE-9171-B65EB8013283}">
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,6 +1337,554 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109"/>
     </row>
@@ -1279,11 +1897,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{880D1DE9-BE6D-4795-80FF-94E1FC3649A9}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{35F02A19-9F16-4723-A355-585FED636D99}">
           <x14:formula1>
-            <xm:f>Totals!#REF!</xm:f>
+            <xm:f>Totals!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>A201:C250 C253 A2:C8 B110:B200 C44:C115 B48:B108 A42:A69 B46 B41:B44 C42 A40:B40 A35:C39 A34 A28:C33 C34 B26:C27 A27 A9 B12 A12:A13 C9:C13 A14:C25 A10:B11 A137:A200 C117:C121 A71:A135 C123:C200</xm:sqref>
+          <xm:sqref>A1 A2:C20 F12 A22:C1048576 A21:B21 C21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1295,7 +1913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6F3C74-44B5-471F-AE13-9C8CA1826F77}">
   <dimension ref="A1:C254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1325,215 +1945,215 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8">
         <f>COUNTIF(History!A:C,A2)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C2" s="8">
         <f>COUNTIF(History!A:A,A2)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B3" s="8">
         <f>COUNTIF(History!A:C,A3)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C3" s="8">
         <f>COUNTIF(History!A:A,A3)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="B4" s="8">
         <f>COUNTIF(History!A:C,A4)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8">
         <f>COUNTIF(History!A:A,A4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="B5" s="8">
         <f>COUNTIF(History!A:C,A5)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8">
         <f>COUNTIF(History!A:A,A5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8">
         <f>COUNTIF(History!A:C,A6)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C6" s="8">
         <f>COUNTIF(History!A:A,A6)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B7" s="8">
         <f>COUNTIF(History!A:C,A7)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C7" s="8">
         <f>COUNTIF(History!A:A,A7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B8" s="8">
         <f>COUNTIF(History!A:C,A8)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="8">
         <f>COUNTIF(History!A:A,A8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="B9" s="8">
         <f>COUNTIF(History!A:C,A9)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C9" s="8">
         <f>COUNTIF(History!A:A,A9)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="B10" s="8">
         <f>COUNTIF(History!A:C,A10)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C10" s="8">
         <f>COUNTIF(History!A:A,A10)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="B11" s="8">
         <f>COUNTIF(History!A:C,A11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11" s="8">
         <f>COUNTIF(History!A:A,A11)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B12" s="8">
         <f>COUNTIF(History!A:C,A12)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C12" s="8">
         <f>COUNTIF(History!A:A,A12)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="B13" s="8">
         <f>COUNTIF(History!A:C,A13)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C13" s="8">
         <f>COUNTIF(History!A:A,A13)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="B14" s="8">
         <f>COUNTIF(History!A:C,A14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="8">
         <f>COUNTIF(History!A:A,A14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B15" s="8">
         <f>COUNTIF(History!A:C,A15)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(History!A:A,A15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B16" s="8">
         <f>COUNTIF(History!A:C,A16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(History!A:A,A16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="B17" s="8">
         <f>COUNTIF(History!A:C,A17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(History!A:A,A17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B18" s="8">
         <f>COUNTIF(History!A:C,A18)</f>
@@ -1546,7 +2166,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="B19" s="8">
         <f>COUNTIF(History!A:C,A19)</f>
@@ -1559,7 +2179,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="B20" s="8">
         <f>COUNTIF(History!A:C,A20)</f>
@@ -1572,7 +2192,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="B21" s="8">
         <f>COUNTIF(History!A:C,A21)</f>
@@ -1585,11 +2205,11 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="B22" s="8">
         <f>COUNTIF(History!A:C,A22)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="8">
         <f>COUNTIF(History!A:A,A22)</f>
@@ -1598,7 +2218,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="B23" s="8">
         <f>COUNTIF(History!A:C,A23)</f>
@@ -1611,7 +2231,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B24" s="8">
         <f>COUNTIF(History!A:C,A24)</f>
@@ -1624,11 +2244,11 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="B25" s="8">
         <f>COUNTIF(History!A:C,A25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="8">
         <f>COUNTIF(History!A:A,A25)</f>
@@ -1637,7 +2257,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B26" s="8">
         <f>COUNTIF(History!A:C,A26)</f>
@@ -1650,7 +2270,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B27" s="8">
         <f>COUNTIF(History!A:C,A27)</f>
@@ -1663,7 +2283,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="8">
         <f>COUNTIF(History!A:C,A28)</f>
@@ -1676,7 +2296,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="B29" s="8">
         <f>COUNTIF(History!A:C,A29)</f>
@@ -1689,11 +2309,11 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="B30" s="8">
         <f>COUNTIF(History!A:C,A30)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30" s="8">
         <f>COUNTIF(History!A:A,A30)</f>
@@ -1702,11 +2322,11 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B31" s="8">
         <f>COUNTIF(History!A:C,A31)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="8">
         <f>COUNTIF(History!A:A,A31)</f>
@@ -1715,7 +2335,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B32" s="8">
         <f>COUNTIF(History!A:C,A32)</f>
@@ -1728,7 +2348,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B33" s="8">
         <f>COUNTIF(History!A:C,A33)</f>
@@ -1741,7 +2361,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="B34" s="8">
         <f>COUNTIF(History!A:C,A34)</f>
@@ -1754,7 +2374,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B35" s="8">
         <f>COUNTIF(History!A:C,A35)</f>
@@ -1767,7 +2387,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="B36" s="8">
         <f>COUNTIF(History!A:C,A36)</f>
@@ -1780,11 +2400,11 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B37" s="8">
         <f>COUNTIF(History!A:C,A37)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="8">
         <f>COUNTIF(History!A:A,A37)</f>
@@ -1793,11 +2413,11 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="B38" s="8">
         <f>COUNTIF(History!A:C,A38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38" s="8">
         <f>COUNTIF(History!A:A,A38)</f>
@@ -1806,7 +2426,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="B39" s="8">
         <f>COUNTIF(History!A:C,A39)</f>
@@ -1819,7 +2439,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="B40" s="8">
         <f>COUNTIF(History!A:C,A40)</f>
@@ -1832,7 +2452,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>123</v>
+        <v>48</v>
       </c>
       <c r="B41" s="8">
         <f>COUNTIF(History!A:C,A41)</f>
@@ -1845,7 +2465,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B42" s="8">
         <f>COUNTIF(History!A:C,A42)</f>
@@ -1858,7 +2478,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="B43" s="8">
         <f>COUNTIF(History!A:C,A43)</f>
@@ -1871,7 +2491,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="B44" s="8">
         <f>COUNTIF(History!A:C,A44)</f>
@@ -1884,7 +2504,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B45" s="8">
         <f>COUNTIF(History!A:C,A45)</f>
@@ -1897,7 +2517,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="B46" s="8">
         <f>COUNTIF(History!A:C,A46)</f>
@@ -1910,7 +2530,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="B47" s="8">
         <f>COUNTIF(History!A:C,A47)</f>
@@ -1923,7 +2543,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="B48" s="8">
         <f>COUNTIF(History!A:C,A48)</f>
@@ -1936,7 +2556,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="B49" s="8">
         <f>COUNTIF(History!A:C,A49)</f>
@@ -1949,7 +2569,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B50" s="8">
         <f>COUNTIF(History!A:C,A50)</f>
@@ -1962,7 +2582,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B51" s="8">
         <f>COUNTIF(History!A:C,A51)</f>
@@ -1975,7 +2595,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="B52" s="8">
         <f>COUNTIF(History!A:C,A52)</f>
@@ -1988,7 +2608,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B53" s="8">
         <f>COUNTIF(History!A:C,A53)</f>
@@ -2001,7 +2621,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="B54" s="8">
         <f>COUNTIF(History!A:C,A54)</f>
@@ -2014,7 +2634,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B55" s="8">
         <f>COUNTIF(History!A:C,A55)</f>
@@ -2027,7 +2647,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B56" s="8">
         <f>COUNTIF(History!A:C,A56)</f>
@@ -2040,7 +2660,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="B57" s="8">
         <f>COUNTIF(History!A:C,A57)</f>
@@ -2053,7 +2673,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B58" s="8">
         <f>COUNTIF(History!A:C,A58)</f>
@@ -2066,7 +2686,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59" s="8">
         <f>COUNTIF(History!A:C,A59)</f>
@@ -2079,7 +2699,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B60" s="8">
         <f>COUNTIF(History!A:C,A60)</f>
@@ -2092,7 +2712,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B61" s="8">
         <f>COUNTIF(History!A:C,A61)</f>
@@ -2105,7 +2725,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B62" s="8">
         <f>COUNTIF(History!A:C,A62)</f>
@@ -2118,7 +2738,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="B63" s="8">
         <f>COUNTIF(History!A:C,A63)</f>
@@ -2131,7 +2751,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B64" s="8">
         <f>COUNTIF(History!A:C,A64)</f>
@@ -2144,7 +2764,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="B65" s="8">
         <f>COUNTIF(History!A:C,A65)</f>
@@ -2157,7 +2777,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="B66" s="8">
         <f>COUNTIF(History!A:C,A66)</f>
@@ -2170,7 +2790,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="B67" s="8">
         <f>COUNTIF(History!A:C,A67)</f>
@@ -2183,7 +2803,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B68" s="8">
         <f>COUNTIF(History!A:C,A68)</f>
@@ -2196,7 +2816,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="B69" s="8">
         <f>COUNTIF(History!A:C,A69)</f>
@@ -2209,7 +2829,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="B70" s="8">
         <f>COUNTIF(History!A:C,A70)</f>
@@ -2222,7 +2842,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B71" s="8">
         <f>COUNTIF(History!A:C,A71)</f>
@@ -2235,7 +2855,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>131</v>
+        <v>38</v>
       </c>
       <c r="B72" s="8">
         <f>COUNTIF(History!A:C,A72)</f>
@@ -2248,7 +2868,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B73" s="8">
         <f>COUNTIF(History!A:C,A73)</f>
@@ -2261,7 +2881,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="B74" s="8">
         <f>COUNTIF(History!A:C,A74)</f>
@@ -2274,7 +2894,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B75" s="8">
         <f>COUNTIF(History!A:C,A75)</f>
@@ -2287,7 +2907,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="B76" s="8">
         <f>COUNTIF(History!A:C,A76)</f>
@@ -2300,7 +2920,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B77" s="8">
         <f>COUNTIF(History!A:C,A77)</f>
@@ -2313,7 +2933,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="B78" s="8">
         <f>COUNTIF(History!A:C,A78)</f>
@@ -2326,7 +2946,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="B79" s="8">
         <f>COUNTIF(History!A:C,A79)</f>
@@ -2339,7 +2959,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="B80" s="8">
         <f>COUNTIF(History!A:C,A80)</f>
@@ -2352,7 +2972,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="B81" s="8">
         <f>COUNTIF(History!A:C,A81)</f>
@@ -2365,7 +2985,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="B82" s="8">
         <f>COUNTIF(History!A:C,A82)</f>
@@ -2378,7 +2998,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B83" s="8">
         <f>COUNTIF(History!A:C,A83)</f>
@@ -2525,7 +3145,7 @@
       </c>
       <c r="B94" s="8">
         <f>COUNTIF(History!A:C,A94)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C94" s="8">
         <f>COUNTIF(History!A:A,A94)</f>
@@ -4614,7 +5234,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{B7BFFF1C-AC35-4424-B8F4-04250131A25E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C122">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C254">
       <sortCondition descending="1" ref="C1"/>
     </sortState>
   </autoFilter>
@@ -4625,10 +5245,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3ACB55-5D50-44AC-A914-44229FBE70D8}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4650,111 +5270,117 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2)</f>
-        <v>giratina_altered:0</v>
+        <v>melmetal:9</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2)</f>
-        <v>giratina_altered:0</v>
+        <v>melmetal:19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3,)</f>
-        <v>giratina_altered:0,dialga:0</v>
+        <v>melmetal:9,kyogre:7</v>
       </c>
       <c r="B3" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3,)</f>
-        <v>giratina_altered:0,dialga:0</v>
+        <v>melmetal:19,kyogre:20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4,)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5</v>
       </c>
       <c r="B4" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5</v>
       </c>
       <c r="B5" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20,metagross:15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4</v>
       </c>
       <c r="B6" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20,metagross:15,togekiss:14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7,)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4,dragonite:3</v>
       </c>
       <c r="B7" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7,)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20,metagross:15,togekiss:14,dragonite:7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8,)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4,dragonite:3,machamp:3</v>
       </c>
       <c r="B8" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!A3, ",",Totals!B4, ":", Totals!A4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8,)</f>
-        <v>giratina_altered:0,dialga:dialga,0:togekiss,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0</v>
+        <v>melmetal:19,kyogre:kyogre,20:dialga,metagross:15,togekiss:14,dragonite:7,machamp:5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4,dragonite:3,machamp:3,mewtwo:2</v>
       </c>
       <c r="B9" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20,metagross:15,togekiss:14,dragonite:7,machamp:5,mewtwo:7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0,kyogre:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4,dragonite:3,machamp:3,mewtwo:2,giratina_origin:2</v>
       </c>
       <c r="B10" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9, ",",Totals!A10, ":", Totals!B10)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0,kyogre:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20,metagross:15,togekiss:14,dragonite:7,machamp:5,mewtwo:7,giratina_origin:8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10, ",",Totals!A11, ":", Totals!C11)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0,kyogre:0,mewtwo:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4,dragonite:3,machamp:3,mewtwo:2,giratina_origin:2,giratina_altered:2</v>
       </c>
       <c r="B11" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9, ",",Totals!A10, ":", Totals!B10, ",",Totals!A11, ":", Totals!B11)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0,kyogre:0,mewtwo:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20,metagross:15,togekiss:14,dragonite:7,machamp:5,mewtwo:7,giratina_origin:8,giratina_altered:3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10, ",",Totals!A11, ":", Totals!C11, ",",Totals!A12, ":", Totals!C12)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0,kyogre:0,mewtwo:0,darkrai:0</v>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4,dragonite:3,machamp:3,mewtwo:2,giratina_origin:2,giratina_altered:2,snorlax:2</v>
       </c>
       <c r="B12" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9, ",",Totals!A10, ":", Totals!B10, ",",Totals!A11, ":", Totals!B11, ",",Totals!A12, ":", Totals!B12)</f>
-        <v>giratina_altered:0,dialga:0,togekiss:0,dragonite_shadow:0,dragonite:0,snorlax_shadow:0,giratina_origin:0,melmetal:0,kyogre:0,mewtwo:0,darkrai:0</v>
+        <v>melmetal:19,kyogre:20,dialga:20,metagross:15,togekiss:14,dragonite:7,machamp:5,mewtwo:7,giratina_origin:8,giratina_altered:3,snorlax:7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10, ",",Totals!A11, ":", Totals!C11, ",",Totals!A12, ":", Totals!C12, ",",Totals!A13, ":", Totals!C13)</f>
+        <v>melmetal:9,kyogre:7,dialga:5,metagross:5,togekiss:4,dragonite:3,machamp:3,mewtwo:2,giratina_origin:2,giratina_altered:2,snorlax:2,swampert:2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating cache/database and adding new database file
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Master - Season 01.xlsx
+++ b/src/main/resources/data/Master - Season 01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpaces\workspace estudo\pokemonGoPvpAnalyzer\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A73BB20-A2DB-4144-9DB6-FFC0789D8DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B50387E-61FC-4324-8B31-BAA37AD4BB02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3840" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{68075319-8292-4D77-A75F-91AD9F2E35E0}"/>
+    <workbookView xWindow="7200" yWindow="3840" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{68075319-8292-4D77-A75F-91AD9F2E35E0}"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="294">
   <si>
     <t>Lead</t>
   </si>
@@ -932,6 +932,9 @@
   </si>
   <si>
     <t>Raikou</t>
+  </si>
+  <si>
+    <t>Latios</t>
   </si>
 </sst>
 </file>
@@ -1344,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CDF088-F31A-4ECE-9171-B65EB8013283}">
-  <dimension ref="A1:D383"/>
+  <dimension ref="A1:D408"/>
   <sheetViews>
-    <sheetView topLeftCell="A352" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A384" sqref="A384"/>
+    <sheetView topLeftCell="A191" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C207" sqref="A2:C207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5517,6 +5520,281 @@
         <v>266</v>
       </c>
     </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A387" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A388" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B389" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B398" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C398" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A399" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B399" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B400" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B401" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A402" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B402" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A403" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A404" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A405" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B405" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A406" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B406" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C406" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A407" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B407" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A408" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B408" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C408" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C334" xr:uid="{7C2C36E3-1530-41A5-9DEB-7401D4EE9E53}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5528,7 +5806,7 @@
           <x14:formula1>
             <xm:f>Totals!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>A1 F12 C206 A2:C205 A206 C215 A207:C214 A215 C274 A274 A216:C273 A275:C1048576</xm:sqref>
+          <xm:sqref>A1 F12 C206 A2:C205 A206 C215 A207:C214 A215 C274 A274 A216:C273 C395 A275:C394 A395 A396:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5540,8 +5818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6F3C74-44B5-471F-AE13-9C8CA1826F77}">
   <dimension ref="A1:C254"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5576,11 +5854,11 @@
       </c>
       <c r="B2" s="8">
         <f>COUNTIF(History!A:C,A2)</f>
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C2" s="8">
         <f>COUNTIF(History!A:A,A2)</f>
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5589,11 +5867,11 @@
       </c>
       <c r="B3" s="8">
         <f>COUNTIF(History!A:C,A3)</f>
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="C3" s="8">
         <f>COUNTIF(History!A:A,A3)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5602,11 +5880,11 @@
       </c>
       <c r="B4" s="8">
         <f>COUNTIF(History!A:C,A4)</f>
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C4" s="8">
         <f>COUNTIF(History!A:A,A4)</f>
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5615,11 +5893,11 @@
       </c>
       <c r="B5" s="8">
         <f>COUNTIF(History!A:C,A5)</f>
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C5" s="8">
         <f>COUNTIF(History!A:A,A5)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5628,11 +5906,11 @@
       </c>
       <c r="B6" s="8">
         <f>COUNTIF(History!A:C,A6)</f>
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C6" s="8">
         <f>COUNTIF(History!A:A,A6)</f>
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5641,11 +5919,11 @@
       </c>
       <c r="B7" s="8">
         <f>COUNTIF(History!A:C,A7)</f>
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C7" s="8">
         <f>COUNTIF(History!A:A,A7)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5654,7 +5932,7 @@
       </c>
       <c r="B8" s="8">
         <f>COUNTIF(History!A:C,A8)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="8">
         <f>COUNTIF(History!A:A,A8)</f>
@@ -5667,7 +5945,7 @@
       </c>
       <c r="B9" s="8">
         <f>COUNTIF(History!A:C,A9)</f>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C9" s="8">
         <f>COUNTIF(History!A:A,A9)</f>
@@ -5680,46 +5958,46 @@
       </c>
       <c r="B10" s="8">
         <f>COUNTIF(History!A:C,A10)</f>
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C10" s="8">
         <f>COUNTIF(History!A:A,A10)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B11" s="8">
         <f>COUNTIF(History!A:C,A11)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C11" s="8">
         <f>COUNTIF(History!A:A,A11)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B12" s="8">
         <f>COUNTIF(History!A:C,A12)</f>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8">
         <f>COUNTIF(History!A:A,A12)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="B13" s="8">
         <f>COUNTIF(History!A:C,A13)</f>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8">
         <f>COUNTIF(History!A:A,A13)</f>
@@ -5771,29 +6049,29 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTIF(History!A:C,A17)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(History!A:A,A17)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B18" s="8">
         <f>COUNTIF(History!A:C,A18)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" s="8">
         <f>COUNTIF(History!A:A,A18)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="B19" s="8">
         <f>COUNTIF(History!A:C,A19)</f>
@@ -6044,7 +6322,7 @@
       </c>
       <c r="B38" s="8">
         <f>COUNTIF(History!A:C,A38)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="8">
         <f>COUNTIF(History!A:A,A38)</f>
@@ -8874,8 +9152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3ACB55-5D50-44AC-A914-44229FBE70D8}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8897,117 +9175,117 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2)</f>
-        <v>melmetal:72</v>
+        <v>melmetal:77</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2)</f>
-        <v>melmetal:169</v>
+        <v>melmetal:177</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3,)</f>
-        <v>melmetal:72,dialga:69</v>
+        <v>melmetal:77,dialga:70</v>
       </c>
       <c r="B3" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3,)</f>
-        <v>melmetal:169,dialga:234</v>
+        <v>melmetal:177,dialga:249</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4,)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66</v>
       </c>
       <c r="B4" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43</v>
       </c>
       <c r="B5" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42</v>
       </c>
       <c r="B6" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113,togekiss:87</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120,togekiss:97</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7,)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37,machamp:17</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42,machamp:20</v>
       </c>
       <c r="B7" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7,)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113,togekiss:87,machamp:44</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120,togekiss:97,machamp:49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8,)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37,machamp:17,rhyperior:15</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42,machamp:20,rhyperior:15</v>
       </c>
       <c r="B8" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8,)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113,togekiss:87,machamp:44,rhyperior:34</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120,togekiss:97,machamp:49,rhyperior:35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37,machamp:17,rhyperior:15,metagross:15</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42,machamp:20,rhyperior:15,metagross:15</v>
       </c>
       <c r="B9" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113,togekiss:87,machamp:44,rhyperior:34,metagross:61</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120,togekiss:97,machamp:49,rhyperior:35,metagross:63</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37,machamp:17,rhyperior:15,metagross:15,snorlax:10</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42,machamp:20,rhyperior:15,metagross:15,snorlax:13</v>
       </c>
       <c r="B10" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9, ",",Totals!A10, ":", Totals!B10)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113,togekiss:87,machamp:44,rhyperior:34,metagross:61,snorlax:74</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120,togekiss:97,machamp:49,rhyperior:35,metagross:63,snorlax:81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10, ",",Totals!A11, ":", Totals!C11)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37,machamp:17,rhyperior:15,metagross:15,snorlax:10,giratina_altered:6</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42,machamp:20,rhyperior:15,metagross:15,snorlax:13,mewtwo:9</v>
       </c>
       <c r="B11" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9, ",",Totals!A10, ":", Totals!B10, ",",Totals!A11, ":", Totals!B11)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113,togekiss:87,machamp:44,rhyperior:34,metagross:61,snorlax:74,giratina_altered:27</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120,togekiss:97,machamp:49,rhyperior:35,metagross:63,snorlax:81,mewtwo:33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10, ",",Totals!A11, ":", Totals!C11, ",",Totals!A12, ":", Totals!C12)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37,machamp:17,rhyperior:15,metagross:15,snorlax:10,giratina_altered:6,mewtwo:8</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42,machamp:20,rhyperior:15,metagross:15,snorlax:13,mewtwo:9,garchomp:7</v>
       </c>
       <c r="B12" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!B2, ",",Totals!A3, ":", Totals!B3, ",",Totals!A4, ":", Totals!B4, ",",Totals!A5, ":", Totals!B5, ",",Totals!A6, ":", Totals!B6, ",",Totals!A7, ":", Totals!B7, ",",Totals!A8, ":", Totals!B8, ",",Totals!A9, ":", Totals!B9, ",",Totals!A10, ":", Totals!B10, ",",Totals!A11, ":", Totals!B11, ",",Totals!A12, ":", Totals!B12)</f>
-        <v>melmetal:169,dialga:234,giratina_origin:140,kyogre:113,togekiss:87,machamp:44,rhyperior:34,metagross:61,snorlax:74,giratina_altered:27,mewtwo:30</v>
+        <v>melmetal:177,dialga:249,giratina_origin:150,kyogre:120,togekiss:97,machamp:49,rhyperior:35,metagross:63,snorlax:81,mewtwo:33,garchomp:24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CONCATENATE(Totals!A2, ":", Totals!C2, ",",Totals!A3, ":", Totals!C3, ",",Totals!A4, ":", Totals!C4, ",",Totals!A5, ":", Totals!C5, ",",Totals!A6, ":", Totals!C6, ",",Totals!A7, ":", Totals!C7, ",",Totals!A8, ":", Totals!C8, ",",Totals!A9, ":", Totals!C9, ",",Totals!A10, ":", Totals!C10, ",",Totals!A11, ":", Totals!C11, ",",Totals!A12, ":", Totals!C12, ",",Totals!A13, ":", Totals!C13)</f>
-        <v>melmetal:72,dialga:69,giratina_origin:64,kyogre:41,togekiss:37,machamp:17,rhyperior:15,metagross:15,snorlax:10,giratina_altered:6,mewtwo:8,garchomp:6</v>
+        <v>melmetal:77,dialga:70,giratina_origin:66,kyogre:43,togekiss:42,machamp:20,rhyperior:15,metagross:15,snorlax:13,mewtwo:9,garchomp:7,giratina_altered:6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>